<commit_message>
write on excel the values for platform
</commit_message>
<xml_diff>
--- a/ExamesMedicos.xlsx
+++ b/ExamesMedicos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2210627\Desktop\Mestrado\AE\2ARTs_EAProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29B8C481-ED7D-4250-8469-67DF9AF9EBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E607E43B-B51C-45F4-819B-7E258D3FFBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9BA3AF86-6851-4C28-B313-FE06080D03AC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Paciente</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Creatinina</t>
   </si>
   <si>
-    <t>T3 Total</t>
-  </si>
-  <si>
     <t>Tiroxina Livre</t>
   </si>
   <si>
@@ -122,6 +119,54 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>Colesterol</t>
+  </si>
+  <si>
+    <t>VANESSA HINSELMANN DOS SANTOS</t>
+  </si>
+  <si>
+    <t>35,90</t>
+  </si>
+  <si>
+    <t>12,00</t>
+  </si>
+  <si>
+    <t>DAVI KOBUS ZORZI</t>
+  </si>
+  <si>
+    <t>39,4</t>
+  </si>
+  <si>
+    <t>13,5</t>
+  </si>
+  <si>
+    <t>NATHALIA MACENA CUSTODIO</t>
+  </si>
+  <si>
+    <t>36,6</t>
+  </si>
+  <si>
+    <t>12,5</t>
+  </si>
+  <si>
+    <t>8,4</t>
+  </si>
+  <si>
+    <t>35,0</t>
+  </si>
+  <si>
+    <t>162,8</t>
+  </si>
+  <si>
+    <t>OLIVIO JUVENCIO DA SILVA</t>
+  </si>
+  <si>
+    <t>41,9</t>
+  </si>
+  <si>
+    <t>14,7</t>
   </si>
 </sst>
 </file>
@@ -473,19 +518,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D952A00-6DD6-403D-8D57-90AD3093E762}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="10" max="10" width="10.88671875" customWidth="1"/>
     <col min="11" max="11" width="9.88671875" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
     <col min="14" max="14" width="11.77734375" customWidth="1"/>
     <col min="15" max="15" width="10.5546875" customWidth="1"/>
     <col min="17" max="17" width="15.6640625" customWidth="1"/>
@@ -503,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -572,19 +619,117 @@
         <v>22</v>
       </c>
       <c r="Y1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="N2">
+        <v>52</v>
+      </c>
+      <c r="S2">
+        <v>4</v>
+      </c>
+      <c r="T2">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3">
+        <v>3.69</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3">
+        <v>243</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4">
+        <v>6.78</v>
+      </c>
+      <c r="N4">
+        <v>66</v>
+      </c>
+      <c r="S4">
+        <v>7</v>
+      </c>
+      <c r="Y4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5">
+        <v>7.46</v>
+      </c>
+      <c r="N5">
         <v>27</v>
+      </c>
+      <c r="S5">
+        <v>10</v>
+      </c>
+      <c r="T5">
+        <v>238</v>
+      </c>
+      <c r="Y5">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
select on platform by name
</commit_message>
<xml_diff>
--- a/ExamesMedicos.xlsx
+++ b/ExamesMedicos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2210627\Desktop\Mestrado\AE\2ARTs_EAProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E607E43B-B51C-45F4-819B-7E258D3FFBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C626A38F-183F-4895-B928-0676B9FC2EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9BA3AF86-6851-4C28-B313-FE06080D03AC}"/>
   </bookViews>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D952A00-6DD6-403D-8D57-90AD3093E762}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>